<commit_message>
Updated CCRL comparison [qa]
</commit_message>
<xml_diff>
--- a/Docs/Floyd on CCRL.xlsx
+++ b/Docs/Floyd on CCRL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="0" windowWidth="23780" windowHeight="16700" tabRatio="500"/>
+    <workbookView xWindow="1420" yWindow="120" windowWidth="13560" windowHeight="16700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Maverick 1.5</t>
   </si>
   <si>
-    <t>Gnuchess 5.60</t>
-  </si>
-  <si>
     <t>ProDeo 1.86</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>List difference</t>
+  </si>
+  <si>
+    <t>Gnu Chesss 5.60</t>
   </si>
 </sst>
 </file>
@@ -249,16 +249,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2045.8</c:v>
+                  <c:v>2046.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2218.8</c:v>
+                  <c:v>2219.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2367.8</c:v>
+                  <c:v>2367.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2542.8</c:v>
+                  <c:v>2542.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -306,13 +306,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="1">
-                  <c:v>2285.2</c:v>
+                  <c:v>2283.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2486.2</c:v>
+                  <c:v>2485.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2658.2</c:v>
+                  <c:v>2640.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -329,11 +329,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2092459176"/>
-        <c:axId val="-2092455192"/>
+        <c:axId val="2098334760"/>
+        <c:axId val="2080309560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2092459176"/>
+        <c:axId val="2098334760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -342,7 +342,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092455192"/>
+        <c:crossAx val="2080309560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -350,7 +350,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2092455192"/>
+        <c:axId val="2080309560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2800.0"/>
@@ -363,7 +363,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2092459176"/>
+        <c:crossAx val="2098334760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -744,18 +744,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -766,24 +766,24 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>2812</v>
+        <v>2811</v>
       </c>
       <c r="C4">
-        <v>2815</v>
+        <v>2817</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>2751</v>
       </c>
       <c r="C5">
-        <v>2702</v>
+        <v>2701</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -794,7 +794,7 @@
         <v>2900</v>
       </c>
       <c r="C6">
-        <v>2905</v>
+        <v>2907</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -802,10 +802,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="C7">
-        <v>2613</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -813,23 +813,23 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>2574</v>
+        <v>2573</v>
       </c>
       <c r="C8">
-        <v>2519</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>AVERAGE(B4:B8)</f>
-        <v>2737.2</v>
+        <v>2736.6</v>
       </c>
       <c r="C9">
         <f>AVERAGE(C4:C8)</f>
-        <v>2710.8</v>
+        <v>2711.4</v>
       </c>
       <c r="E9">
         <v>2700</v>
@@ -837,7 +837,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -848,7 +848,7 @@
         <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -864,7 +864,7 @@
       </c>
       <c r="F12">
         <f>B12-B$9+$E$9</f>
-        <v>2045.8000000000002</v>
+        <v>2046.4</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -875,7 +875,7 @@
         <v>2256</v>
       </c>
       <c r="C13">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="E13" t="str">
         <f>A13</f>
@@ -883,15 +883,15 @@
       </c>
       <c r="F13">
         <f>B13-B$9+$E$9</f>
-        <v>2218.8000000000002</v>
+        <v>2219.4</v>
       </c>
       <c r="G13">
         <f>C13-C$9+$E$9</f>
-        <v>2285.1999999999998</v>
+        <v>2283.6</v>
       </c>
       <c r="H13">
         <f>G13-F13</f>
-        <v>66.399999999999636</v>
+        <v>64.199999999999818</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -899,7 +899,7 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="C14">
         <v>2497</v>
@@ -910,15 +910,15 @@
       </c>
       <c r="F14">
         <f>B14-B$9+$E$9</f>
-        <v>2367.8000000000002</v>
+        <v>2367.4</v>
       </c>
       <c r="G14">
         <f>C14-C$9+$E$9</f>
-        <v>2486.1999999999998</v>
+        <v>2485.6</v>
       </c>
       <c r="H14">
         <f>G14-F14</f>
-        <v>118.39999999999964</v>
+        <v>118.19999999999982</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -926,10 +926,10 @@
         <v>3</v>
       </c>
       <c r="B15">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="C15">
-        <v>2669</v>
+        <v>2652</v>
       </c>
       <c r="E15" t="str">
         <f>A15</f>
@@ -937,15 +937,15 @@
       </c>
       <c r="F15">
         <f>B15-B$9+$E$9</f>
-        <v>2542.8000000000002</v>
+        <v>2542.4</v>
       </c>
       <c r="G15">
         <f>C15-C$9+$E$9</f>
-        <v>2658.2</v>
+        <v>2640.6</v>
       </c>
       <c r="H15">
         <f>G15-F15</f>
-        <v>115.39999999999964</v>
+        <v>98.199999999999818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>